<commit_message>
added the whole numerics chapter
</commit_message>
<xml_diff>
--- a/simulation_results.xlsx
+++ b/simulation_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjeko\Desktop\TUM-MS\Master Thesis\Simulations\rand_and_diff_eq_in_the_context_of_the_sig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE0AA52-9963-4CAE-8300-E497C1BBB8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234DFBF4-E92F-4378-AFA4-4BE954B076A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AB74C585-8EF9-4162-A044-4B9EFCC45C9E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AB74C585-8EF9-4162-A044-4B9EFCC45C9E}"/>
   </bookViews>
   <sheets>
     <sheet name="double_well_process" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>k =</t>
   </si>
@@ -64,6 +64,39 @@
   </si>
   <si>
     <t>arctan</t>
+  </si>
+  <si>
+    <t>N_test is always 100</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2+x3</t>
+  </si>
+  <si>
+    <t>x1*x4</t>
+  </si>
+  <si>
+    <t>sin(x3^2)</t>
+  </si>
+  <si>
+    <t>x1^2+x3^3</t>
+  </si>
+  <si>
+    <t>x2^2*cos(x4)</t>
+  </si>
+  <si>
+    <t>stronger reg. helps with polynomials</t>
+  </si>
+  <si>
+    <t>all visuals with k=200</t>
+  </si>
+  <si>
+    <t>N_sim = 10000</t>
+  </si>
+  <si>
+    <t>lambda_ridge = 0.001</t>
   </si>
 </sst>
 </file>
@@ -72,7 +105,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -126,12 +159,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -447,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0690CF-4D41-4A95-9197-2809504D4B75}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,120 +521,120 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>2.9293373157024199E-4</v>
+      <c r="B2" s="5">
+        <v>1.9127749413486599E-3</v>
       </c>
       <c r="C2" s="4">
-        <v>2.57119408192123E-4</v>
+        <v>3.8262568253942498E-4</v>
       </c>
       <c r="D2" s="3">
-        <v>1.0521331100680801E-3</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.9373822994651099E-3</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2.2413645414961899E-3</v>
+        <v>1.40957305497284E-3</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1.53601248972944E-3</v>
+      </c>
+      <c r="F2" s="5">
+        <v>3.6485348758130299E-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.16355483713775101</v>
-      </c>
-      <c r="C3" s="2">
-        <v>7.8415697303550594E-2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>9.2576674964598094E-2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>7.6258469069001203E-2</v>
-      </c>
-      <c r="F3" s="4">
-        <v>6.3139628602903203E-2</v>
+      <c r="B3" s="5">
+        <v>0.191620586357372</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.21969574948745199</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.14172177894090901</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.16072361116403699</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.296110056387408</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.175028108551573</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.111268013835939</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2.4567367898660999E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.16426269799475299</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.219637474163179</v>
+      <c r="B4" s="4">
+        <v>0.334856942992458</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.41289613874345099</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.35576084392610502</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.35205203113970501</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.55183986788327399</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
-        <v>4.0197204189961602E-2</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.10318771070251199</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4.3821144383242999E-2</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3.73893334504663E-2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>5.7233079703854203E-2</v>
+      <c r="B5" s="5">
+        <v>6.0289747115905297E-2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3.99977663946798E-2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4.31323547492646E-2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5.3409077460399801E-2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5.8933153502932101E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
-        <v>9.7911200366111506E-2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5.3388666673852697E-2</v>
-      </c>
-      <c r="D6" s="4">
-        <v>5.0066257409284401E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.161235592118772</v>
-      </c>
-      <c r="F6" s="2">
-        <v>5.3572137827480902E-2</v>
+      <c r="B6" s="5">
+        <v>8.6264545513040594E-2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8.5160310287376501E-2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8.8713579510308893E-2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8.8195828983676505E-2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.114324191742518</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2">
-        <v>5.4761946122681503E-2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4.0111491719482403E-2</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2.55116315543501E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5.2181174979775501E-2</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2.4567367898660999E-2</v>
+      <c r="B7" s="4">
+        <v>5.35295054711694E-2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>5.49811973670409E-2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>5.7456649109695598E-2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>6.4733827018239404E-2</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5.9465958133931102E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -622,7 +656,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -631,6 +665,9 @@
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -643,6 +680,16 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -652,14 +699,239 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76580B2-DA62-4B4E-9C17-BFFCAD4B7435}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.201115257967457</v>
+      </c>
+      <c r="C2" s="5">
+        <v>7.7864105952292706E-2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>8.6733502243812502E-2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>8.1460563110185194E-2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3.1873091135373802E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.19722415290385401</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.115083970206998</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.119467546802367</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8.0168968984410893E-2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>8.48744487135729E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1.03909102164673</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.604807625360547</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.52657731631982596</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.57860225242264296</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.56028806687878996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.76575854780637098</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.71573555251520604</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.75114493326409104</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.75853676410572801</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.88073816453741605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.71635927041883296</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.90234509014670194</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.94317917712312205</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.94097600997217501</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1.1249666881287399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1.08012474005805</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.17669112806545</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.89130353849773403</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1.22568484441374</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1.0844783506537701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>250</v>
+      </c>
+      <c r="C18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>0.51039041952523201</v>
+      </c>
+      <c r="C19">
+        <v>0.33768127811327298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>0.57301633134027796</v>
+      </c>
+      <c r="C20">
+        <v>0.77582304573204797</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>0.73665709925312695</v>
+      </c>
+      <c r="C21">
+        <v>0.79862020205151896</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final touches - saturday morning
</commit_message>
<xml_diff>
--- a/simulation_results.xlsx
+++ b/simulation_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjeko\Desktop\TUM-MS\Master Thesis\Simulations\rand_and_diff_eq_in_the_context_of_the_sig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234DFBF4-E92F-4378-AFA4-4BE954B076A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B777819-0C45-48FF-B2CD-558B56C55EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AB74C585-8EF9-4162-A044-4B9EFCC45C9E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>k =</t>
   </si>
@@ -159,13 +159,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -702,7 +703,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C19" sqref="C19:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -871,9 +872,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18">
@@ -887,10 +886,10 @@
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>0.51039041952523201</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>0.33768127811327298</v>
       </c>
     </row>
@@ -898,10 +897,10 @@
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="6">
         <v>0.57301633134027796</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>0.77582304573204797</v>
       </c>
     </row>
@@ -909,10 +908,10 @@
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="6">
         <v>0.73665709925312695</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>0.79862020205151896</v>
       </c>
     </row>
@@ -920,6 +919,12 @@
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B22" s="6">
+        <v>0.79070413258234695</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.81894339152506601</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -933,5 +938,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>